<commit_message>
waterquality sangju 2020 <--del
</commit_message>
<xml_diff>
--- a/data/nak/수질/상주2_2020.xlsx
+++ b/data/nak/수질/상주2_2020.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\사업관련\환경AI\모듈작업\water-quality\data\nak\수질\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="122">
   <si>
     <t>dt</t>
   </si>
@@ -378,77 +385,36 @@
   </si>
   <si>
     <t>20200706</t>
-  </si>
-  <si>
-    <t>2020-07-16 12:00</t>
-  </si>
-  <si>
-    <t>20200715</t>
-  </si>
-  <si>
-    <t>2020-07-24 12:00</t>
-  </si>
-  <si>
-    <t>20200720</t>
-  </si>
-  <si>
-    <t>2020-08-10 12:00</t>
-  </si>
-  <si>
-    <t>20200818</t>
-  </si>
-  <si>
-    <t>2020-08-20 12:00</t>
-  </si>
-  <si>
-    <t>20200825</t>
-  </si>
-  <si>
-    <t>2020-09-06 12:00</t>
-  </si>
-  <si>
-    <t>20200901</t>
-  </si>
-  <si>
-    <t>2020-09-12 12:00</t>
-  </si>
-  <si>
-    <t>20200909</t>
-  </si>
-  <si>
-    <t>2020-09-18 12:00</t>
-  </si>
-  <si>
-    <t>20200914</t>
-  </si>
-  <si>
-    <t>2020-09-24 12:00</t>
-  </si>
-  <si>
-    <t>20200922</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="0.000000"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="0.000000"/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="178" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -466,7 +432,13 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -474,16 +446,24 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -492,10 +472,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -741,83 +721,79 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
+  <dimension ref="A1:BJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.43" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.86" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.57" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.71" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.75" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.75" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.75" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.75" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.75" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.75" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.43" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.71" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.75" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.71" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.71" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.71" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="4.29" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.43" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.43" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.43" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="6.57" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="6.57" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.43" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.43" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.86" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="6.71" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="6.57" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="6.57" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="4.71" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.43" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.43" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="8.86" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.86" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.43" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.14" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8.29" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.86" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8.43" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="8.43" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="10.14" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="10.14" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="18.57" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.43" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="9.71" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.71" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="9.43" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="4.75" bestFit="1" customWidth="1"/>
+    <col min="46" max="47" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="56" max="57" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1005,7 +981,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -1082,13 +1058,13 @@
         <v>78</v>
       </c>
       <c r="AC2" s="3">
-        <v>0.092999999999999999</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="AD2" s="3">
         <v>2.456</v>
       </c>
       <c r="AE2" s="4">
-        <v>7.9000000000000004</v>
+        <v>7.9</v>
       </c>
       <c r="AF2">
         <v>5</v>
@@ -1100,7 +1076,7 @@
         <v>1.3</v>
       </c>
       <c r="AI2" s="4">
-        <v>14.199999999999999</v>
+        <v>14.2</v>
       </c>
       <c r="AJ2" s="4">
         <v>12.9</v>
@@ -1109,28 +1085,28 @@
         <v>3.2440000000000002</v>
       </c>
       <c r="AL2" s="3">
-        <v>0.051999999999999998</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="AN2" s="4">
-        <v>4.7999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="AO2" s="4">
         <v>4.5</v>
       </c>
       <c r="AP2" s="3">
-        <v>0.028000000000000001</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="AQ2" s="3">
         <v>3.1619999999999999</v>
       </c>
       <c r="AR2" s="3">
-        <v>0.041000000000000002</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="AS2" s="4">
-        <v>3.8999999999999999</v>
+        <v>3.9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -1207,25 +1183,25 @@
         <v>81</v>
       </c>
       <c r="AC3" s="3">
-        <v>0.064000000000000001</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AD3" s="3">
         <v>2.8580000000000001</v>
       </c>
       <c r="AE3" s="4">
-        <v>8.0999999999999996</v>
+        <v>8.1</v>
       </c>
       <c r="AF3" s="4">
-        <v>3.8999999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="AG3">
         <v>222</v>
       </c>
       <c r="AH3" s="4">
-        <v>0.69999999999999996</v>
+        <v>0.7</v>
       </c>
       <c r="AI3" s="4">
-        <v>4.2000000000000002</v>
+        <v>4.2</v>
       </c>
       <c r="AJ3" s="4">
         <v>13.5</v>
@@ -1234,25 +1210,25 @@
         <v>3.0950000000000002</v>
       </c>
       <c r="AL3" s="3">
-        <v>0.032000000000000001</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="AN3" s="4">
-        <v>4.7000000000000002</v>
+        <v>4.7</v>
       </c>
       <c r="AO3" s="4">
         <v>4.4000000000000004</v>
       </c>
       <c r="AP3" s="3">
-        <v>0.010999999999999999</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="AQ3" s="5">
-        <v>3.0899999999999999</v>
+        <v>3.09</v>
       </c>
       <c r="AR3" s="3">
-        <v>0.025999999999999999</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -1329,13 +1305,13 @@
         <v>84</v>
       </c>
       <c r="AC4" s="3">
-        <v>0.042999999999999997</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="AD4" s="3">
         <v>2.4630000000000001</v>
       </c>
       <c r="AE4" s="4">
-        <v>8.0999999999999996</v>
+        <v>8.1</v>
       </c>
       <c r="AF4" s="4">
         <v>3.5</v>
@@ -1347,7 +1323,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AI4" s="4">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AJ4" s="4">
         <v>13.6</v>
@@ -1356,7 +1332,7 @@
         <v>3.391</v>
       </c>
       <c r="AL4" s="3">
-        <v>0.023</v>
+        <v>2.3E-2</v>
       </c>
       <c r="AN4" s="4">
         <v>4.9000000000000004</v>
@@ -1365,16 +1341,16 @@
         <v>5.5</v>
       </c>
       <c r="AP4" s="3">
-        <v>0.0040000000000000001</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AQ4" s="3">
         <v>3.1709999999999998</v>
       </c>
       <c r="AR4" s="3">
-        <v>0.017999999999999999</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1451,7 +1427,7 @@
         <v>86</v>
       </c>
       <c r="AC5" s="3">
-        <v>0.025000000000000001</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AD5" s="3">
         <v>2.6949999999999998</v>
@@ -1460,7 +1436,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="AF5" s="4">
-        <v>3.8999999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="AG5">
         <v>251</v>
@@ -1478,10 +1454,10 @@
         <v>3.3540000000000001</v>
       </c>
       <c r="AL5" s="3">
-        <v>0.024</v>
+        <v>2.4E-2</v>
       </c>
       <c r="AN5" s="4">
-        <v>6.5999999999999996</v>
+        <v>6.6</v>
       </c>
       <c r="AO5" s="4">
         <v>14.6</v>
@@ -1493,13 +1469,13 @@
         <v>3.3479999999999999</v>
       </c>
       <c r="AR5" s="3">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="AS5" s="4">
-        <v>2.8999999999999999</v>
+        <v>2.9</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1576,7 +1552,7 @@
         <v>88</v>
       </c>
       <c r="AC6" s="3">
-        <v>0.025999999999999999</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="AD6" s="3">
         <v>2.2930000000000001</v>
@@ -1591,7 +1567,7 @@
         <v>232</v>
       </c>
       <c r="AH6" s="4">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="AI6">
         <v>6</v>
@@ -1600,16 +1576,16 @@
         <v>14.5</v>
       </c>
       <c r="AK6" s="5">
-        <v>2.6699999999999999</v>
+        <v>2.67</v>
       </c>
       <c r="AL6" s="3">
-        <v>0.021999999999999999</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="AN6" s="4">
         <v>5.5</v>
       </c>
       <c r="AO6" s="4">
-        <v>27.100000000000001</v>
+        <v>27.1</v>
       </c>
       <c r="AP6">
         <v>0</v>
@@ -1618,10 +1594,10 @@
         <v>2.657</v>
       </c>
       <c r="AR6" s="3">
-        <v>0.012999999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -1698,7 +1674,7 @@
         <v>90</v>
       </c>
       <c r="AC7" s="3">
-        <v>0.094</v>
+        <v>9.4E-2</v>
       </c>
       <c r="AD7" s="3">
         <v>1.7589999999999999</v>
@@ -1719,13 +1695,13 @@
         <v>19.600000000000001</v>
       </c>
       <c r="AJ7" s="4">
-        <v>12.800000000000001</v>
+        <v>12.8</v>
       </c>
       <c r="AK7" s="3">
         <v>2.7730000000000001</v>
       </c>
       <c r="AL7" s="3">
-        <v>0.050999999999999997</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="AN7" s="4">
         <v>8.8000000000000007</v>
@@ -1734,16 +1710,16 @@
         <v>18.600000000000001</v>
       </c>
       <c r="AP7" s="3">
-        <v>0.0050000000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AQ7" s="3">
         <v>2.6619999999999999</v>
       </c>
       <c r="AR7" s="3">
-        <v>0.017999999999999999</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1820,16 +1796,16 @@
         <v>92</v>
       </c>
       <c r="AC8" s="3">
-        <v>0.027</v>
+        <v>2.7E-2</v>
       </c>
       <c r="AD8" s="3">
         <v>2.6749999999999998</v>
       </c>
       <c r="AE8" s="4">
-        <v>8.0999999999999996</v>
+        <v>8.1</v>
       </c>
       <c r="AF8" s="4">
-        <v>4.2999999999999998</v>
+        <v>4.3</v>
       </c>
       <c r="AG8">
         <v>201</v>
@@ -1838,7 +1814,7 @@
         <v>1.5</v>
       </c>
       <c r="AI8" s="4">
-        <v>5.7999999999999998</v>
+        <v>5.8</v>
       </c>
       <c r="AJ8" s="4">
         <v>12.4</v>
@@ -1847,7 +1823,7 @@
         <v>3.0350000000000001</v>
       </c>
       <c r="AL8" s="3">
-        <v>0.023</v>
+        <v>2.3E-2</v>
       </c>
       <c r="AN8" s="4">
         <v>9.1999999999999993</v>
@@ -1856,19 +1832,19 @@
         <v>17</v>
       </c>
       <c r="AP8" s="3">
-        <v>0.0030000000000000001</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AQ8" s="3">
         <v>2.9750000000000001</v>
       </c>
       <c r="AR8" s="3">
-        <v>0.012999999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="AS8" s="4">
         <v>3.5</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -1945,13 +1921,13 @@
         <v>94</v>
       </c>
       <c r="AC9" s="3">
-        <v>0.028000000000000001</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="AD9" s="3">
         <v>2.4929999999999999</v>
       </c>
       <c r="AE9" s="4">
-        <v>8.0999999999999996</v>
+        <v>8.1</v>
       </c>
       <c r="AF9" s="4">
         <v>4.5</v>
@@ -1960,7 +1936,7 @@
         <v>221</v>
       </c>
       <c r="AH9" s="4">
-        <v>1.3999999999999999</v>
+        <v>1.4</v>
       </c>
       <c r="AI9" s="4">
         <v>8.1999999999999993</v>
@@ -1972,25 +1948,25 @@
         <v>2.754</v>
       </c>
       <c r="AL9" s="3">
-        <v>0.021000000000000001</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AN9" s="4">
-        <v>9.4000000000000004</v>
+        <v>9.4</v>
       </c>
       <c r="AO9" s="4">
         <v>19.399999999999999</v>
       </c>
       <c r="AP9" s="3">
-        <v>0.0030000000000000001</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AQ9" s="3">
         <v>2.6789999999999998</v>
       </c>
       <c r="AR9" s="3">
-        <v>0.0070000000000000001</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -2067,7 +2043,7 @@
         <v>96</v>
       </c>
       <c r="AC10" s="3">
-        <v>0.017000000000000001</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="AD10" s="3">
         <v>2.2410000000000001</v>
@@ -2076,7 +2052,7 @@
         <v>8.5</v>
       </c>
       <c r="AF10" s="4">
-        <v>3.7999999999999998</v>
+        <v>3.8</v>
       </c>
       <c r="AG10">
         <v>233</v>
@@ -2085,7 +2061,7 @@
         <v>1.3</v>
       </c>
       <c r="AI10" s="4">
-        <v>3.7999999999999998</v>
+        <v>3.8</v>
       </c>
       <c r="AJ10">
         <v>12</v>
@@ -2094,25 +2070,25 @@
         <v>2.9159999999999999</v>
       </c>
       <c r="AL10" s="3">
-        <v>0.023</v>
+        <v>2.3E-2</v>
       </c>
       <c r="AN10" s="4">
         <v>13.4</v>
       </c>
       <c r="AO10" s="4">
-        <v>3.8999999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="AP10" s="3">
-        <v>0.0040000000000000001</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AQ10" s="3">
         <v>2.7440000000000002</v>
       </c>
       <c r="AR10" s="3">
-        <v>0.012999999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>97</v>
       </c>
@@ -2189,13 +2165,13 @@
         <v>98</v>
       </c>
       <c r="AC11" s="3">
-        <v>0.025000000000000001</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AD11" s="3">
         <v>1.8979999999999999</v>
       </c>
       <c r="AE11" s="4">
-        <v>8.0999999999999996</v>
+        <v>8.1</v>
       </c>
       <c r="AF11" s="4">
         <v>4.0999999999999996</v>
@@ -2207,16 +2183,16 @@
         <v>1.5</v>
       </c>
       <c r="AI11" s="4">
-        <v>4.2000000000000002</v>
+        <v>4.2</v>
       </c>
       <c r="AJ11" s="4">
-        <v>11.199999999999999</v>
+        <v>11.2</v>
       </c>
       <c r="AK11" s="3">
         <v>2.2559999999999998</v>
       </c>
       <c r="AL11" s="3">
-        <v>0.021000000000000001</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AN11" s="4">
         <v>14.9</v>
@@ -2225,19 +2201,19 @@
         <v>11.9</v>
       </c>
       <c r="AP11" s="3">
-        <v>0.0030000000000000001</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AQ11" s="3">
         <v>2.1320000000000001</v>
       </c>
       <c r="AR11" s="3">
-        <v>0.014999999999999999</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AS11" s="4">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>99</v>
       </c>
@@ -2314,7 +2290,7 @@
         <v>100</v>
       </c>
       <c r="AC12" s="3">
-        <v>0.043999999999999997</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="AD12" s="3">
         <v>1.7929999999999999</v>
@@ -2323,7 +2299,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="AF12" s="4">
-        <v>4.2000000000000002</v>
+        <v>4.2</v>
       </c>
       <c r="AG12">
         <v>248</v>
@@ -2332,7 +2308,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="AI12" s="4">
-        <v>4.7999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="AJ12" s="4">
         <v>11.1</v>
@@ -2341,25 +2317,25 @@
         <v>2.052</v>
       </c>
       <c r="AL12" s="3">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="AN12" s="4">
-        <v>15.699999999999999</v>
+        <v>15.7</v>
       </c>
       <c r="AO12" s="4">
         <v>13.4</v>
       </c>
       <c r="AP12" s="3">
-        <v>0.0050000000000000001</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AQ12" s="3">
         <v>2.0390000000000001</v>
       </c>
       <c r="AR12" s="3">
-        <v>0.012999999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>101</v>
       </c>
@@ -2436,7 +2412,7 @@
         <v>102</v>
       </c>
       <c r="AC13" s="3">
-        <v>0.037999999999999999</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="AD13" s="3">
         <v>1.6160000000000001</v>
@@ -2445,7 +2421,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="AF13" s="4">
-        <v>4.2000000000000002</v>
+        <v>4.2</v>
       </c>
       <c r="AG13">
         <v>245</v>
@@ -2466,7 +2442,7 @@
         <v>0.02</v>
       </c>
       <c r="AN13" s="4">
-        <v>14.699999999999999</v>
+        <v>14.7</v>
       </c>
       <c r="AO13" s="4">
         <v>11.9</v>
@@ -2475,13 +2451,13 @@
         <v>0</v>
       </c>
       <c r="AQ13" s="5">
-        <v>1.9199999999999999</v>
+        <v>1.92</v>
       </c>
       <c r="AR13" s="3">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -2558,7 +2534,7 @@
         <v>104</v>
       </c>
       <c r="AC14" s="3">
-        <v>0.028000000000000001</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="AD14" s="3">
         <v>1.2609999999999999</v>
@@ -2567,7 +2543,7 @@
         <v>8.5</v>
       </c>
       <c r="AF14" s="4">
-        <v>5.2999999999999998</v>
+        <v>5.3</v>
       </c>
       <c r="AG14">
         <v>256</v>
@@ -2576,7 +2552,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="AI14" s="4">
-        <v>5.5999999999999996</v>
+        <v>5.6</v>
       </c>
       <c r="AJ14" s="4">
         <v>9.8000000000000007</v>
@@ -2585,13 +2561,13 @@
         <v>1.6879999999999999</v>
       </c>
       <c r="AL14" s="3">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="AN14" s="4">
         <v>20.399999999999999</v>
       </c>
       <c r="AO14" s="4">
-        <v>6.2999999999999998</v>
+        <v>6.3</v>
       </c>
       <c r="AP14">
         <v>0</v>
@@ -2600,10 +2576,10 @@
         <v>1.6719999999999999</v>
       </c>
       <c r="AR14" s="3">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -2680,13 +2656,13 @@
         <v>106</v>
       </c>
       <c r="AC15" s="3">
-        <v>0.067000000000000004</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="AD15" s="3">
         <v>1.179</v>
       </c>
       <c r="AE15" s="4">
-        <v>7.5999999999999996</v>
+        <v>7.6</v>
       </c>
       <c r="AF15" s="4">
         <v>4.5999999999999996</v>
@@ -2698,7 +2674,7 @@
         <v>1.8</v>
       </c>
       <c r="AI15" s="4">
-        <v>3.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="AJ15" s="4">
         <v>9.3000000000000007</v>
@@ -2707,28 +2683,28 @@
         <v>1.6539999999999999</v>
       </c>
       <c r="AL15" s="3">
-        <v>0.031</v>
+        <v>3.1E-2</v>
       </c>
       <c r="AN15" s="4">
         <v>19.600000000000001</v>
       </c>
       <c r="AO15" s="4">
-        <v>9.0999999999999996</v>
+        <v>9.1</v>
       </c>
       <c r="AP15" s="3">
-        <v>0.0030000000000000001</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AQ15" s="3">
         <v>1.615</v>
       </c>
       <c r="AR15" s="3">
-        <v>0.017999999999999999</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="AS15" s="4">
-        <v>3.8999999999999999</v>
+        <v>3.9</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -2811,7 +2787,7 @@
         <v>1.2410000000000001</v>
       </c>
       <c r="AE16" s="4">
-        <v>7.2000000000000002</v>
+        <v>7.2</v>
       </c>
       <c r="AF16" s="4">
         <v>5.0999999999999996</v>
@@ -2823,34 +2799,34 @@
         <v>1.5</v>
       </c>
       <c r="AI16" s="4">
-        <v>4.7999999999999998</v>
+        <v>4.8</v>
       </c>
       <c r="AJ16" s="4">
-        <v>9.0999999999999996</v>
+        <v>9.1</v>
       </c>
       <c r="AK16" s="3">
         <v>1.9419999999999999</v>
       </c>
       <c r="AL16" s="3">
-        <v>0.024</v>
+        <v>2.4E-2</v>
       </c>
       <c r="AN16" s="4">
         <v>21.5</v>
       </c>
       <c r="AO16" s="4">
-        <v>9.4000000000000004</v>
+        <v>9.4</v>
       </c>
       <c r="AP16" s="3">
-        <v>0.0070000000000000001</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AQ16" s="3">
         <v>1.9410000000000001</v>
       </c>
       <c r="AR16" s="3">
-        <v>0.017999999999999999</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -2927,25 +2903,25 @@
         <v>111</v>
       </c>
       <c r="AC17" s="3">
-        <v>0.027</v>
+        <v>2.7E-2</v>
       </c>
       <c r="AD17" s="3">
         <v>1.6160000000000001</v>
       </c>
       <c r="AE17" s="4">
-        <v>8.4000000000000004</v>
+        <v>8.4</v>
       </c>
       <c r="AF17" s="4">
-        <v>7.5999999999999996</v>
+        <v>7.6</v>
       </c>
       <c r="AG17">
         <v>218</v>
       </c>
       <c r="AH17" s="4">
-        <v>2.7999999999999998</v>
+        <v>2.8</v>
       </c>
       <c r="AI17" s="4">
-        <v>8.4000000000000004</v>
+        <v>8.4</v>
       </c>
       <c r="AJ17">
         <v>11</v>
@@ -2954,25 +2930,25 @@
         <v>2.3719999999999999</v>
       </c>
       <c r="AL17" s="3">
-        <v>0.044999999999999998</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="AN17">
         <v>23</v>
       </c>
       <c r="AO17" s="4">
-        <v>41.899999999999999</v>
+        <v>41.9</v>
       </c>
       <c r="AP17" s="3">
-        <v>0.0030000000000000001</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AQ17" s="3">
         <v>2.3580000000000001</v>
       </c>
       <c r="AR17" s="3">
-        <v>0.031</v>
+        <v>3.1E-2</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>112</v>
       </c>
@@ -3049,7 +3025,7 @@
         <v>113</v>
       </c>
       <c r="AC18" s="3">
-        <v>0.066000000000000003</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="AD18" s="3">
         <v>1.333</v>
@@ -3058,13 +3034,13 @@
         <v>8.5</v>
       </c>
       <c r="AF18" s="4">
-        <v>5.4000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="AG18">
         <v>217</v>
       </c>
       <c r="AH18" s="4">
-        <v>2.1000000000000001</v>
+        <v>2.1</v>
       </c>
       <c r="AI18">
         <v>6</v>
@@ -3076,13 +3052,13 @@
         <v>1.988</v>
       </c>
       <c r="AL18" s="3">
-        <v>0.025000000000000001</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AN18" s="4">
-        <v>22.899999999999999</v>
+        <v>22.9</v>
       </c>
       <c r="AO18" s="4">
-        <v>20.899999999999999</v>
+        <v>20.9</v>
       </c>
       <c r="AP18">
         <v>0</v>
@@ -3091,10 +3067,10 @@
         <v>1.9490000000000001</v>
       </c>
       <c r="AR18" s="3">
-        <v>0.017999999999999999</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -3171,16 +3147,16 @@
         <v>115</v>
       </c>
       <c r="AC19" s="3">
-        <v>0.033000000000000002</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="AD19" s="3">
         <v>1.0609999999999999</v>
       </c>
       <c r="AE19" s="4">
-        <v>8.5999999999999996</v>
+        <v>8.6</v>
       </c>
       <c r="AF19" s="4">
-        <v>6.2000000000000002</v>
+        <v>6.2</v>
       </c>
       <c r="AG19">
         <v>240</v>
@@ -3192,34 +3168,34 @@
         <v>4</v>
       </c>
       <c r="AJ19" s="4">
-        <v>8.9000000000000004</v>
+        <v>8.9</v>
       </c>
       <c r="AK19" s="3">
         <v>1.5880000000000001</v>
       </c>
       <c r="AL19" s="3">
-        <v>0.023</v>
+        <v>2.3E-2</v>
       </c>
       <c r="AN19" s="4">
-        <v>29.100000000000001</v>
+        <v>29.1</v>
       </c>
       <c r="AO19" s="4">
         <v>8.5</v>
       </c>
       <c r="AP19" s="3">
-        <v>0.0040000000000000001</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AQ19" s="5">
-        <v>1.5800000000000001</v>
+        <v>1.58</v>
       </c>
       <c r="AR19" s="3">
-        <v>0.017000000000000001</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="AS19" s="4">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>116</v>
       </c>
@@ -3302,10 +3278,10 @@
         <v>1.0049999999999999</v>
       </c>
       <c r="AE20" s="4">
-        <v>7.4000000000000004</v>
+        <v>7.4</v>
       </c>
       <c r="AF20" s="4">
-        <v>6.5999999999999996</v>
+        <v>6.6</v>
       </c>
       <c r="AG20">
         <v>217</v>
@@ -3314,34 +3290,34 @@
         <v>2</v>
       </c>
       <c r="AI20" s="4">
-        <v>8.4000000000000004</v>
+        <v>8.4</v>
       </c>
       <c r="AJ20" s="4">
-        <v>7.5999999999999996</v>
+        <v>7.6</v>
       </c>
       <c r="AK20" s="3">
         <v>1.6419999999999999</v>
       </c>
       <c r="AL20" s="3">
-        <v>0.052999999999999999</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="AN20" s="4">
-        <v>25.800000000000001</v>
+        <v>25.8</v>
       </c>
       <c r="AO20" s="4">
-        <v>6.5999999999999996</v>
+        <v>6.6</v>
       </c>
       <c r="AP20" s="3">
-        <v>0.031</v>
+        <v>3.1E-2</v>
       </c>
       <c r="AQ20" s="3">
         <v>1.635</v>
       </c>
       <c r="AR20" s="3">
-        <v>0.047</v>
+        <v>4.7E-2</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>118</v>
       </c>
@@ -3418,16 +3394,16 @@
         <v>119</v>
       </c>
       <c r="AC21" s="3">
-        <v>0.058000000000000003</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="AD21" s="3">
         <v>0.99299999999999999</v>
       </c>
       <c r="AE21" s="4">
-        <v>8.4000000000000004</v>
+        <v>8.4</v>
       </c>
       <c r="AF21" s="4">
-        <v>6.9000000000000004</v>
+        <v>6.9</v>
       </c>
       <c r="AG21">
         <v>241</v>
@@ -3436,7 +3412,7 @@
         <v>1.5</v>
       </c>
       <c r="AI21" s="4">
-        <v>2.3999999999999999</v>
+        <v>2.4</v>
       </c>
       <c r="AJ21" s="4">
         <v>8.5</v>
@@ -3445,10 +3421,10 @@
         <v>1.6539999999999999</v>
       </c>
       <c r="AL21" s="5">
-        <v>0.040000000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="AN21" s="4">
-        <v>28.100000000000001</v>
+        <v>28.1</v>
       </c>
       <c r="AO21" s="4">
         <v>1.8</v>
@@ -3460,10 +3436,10 @@
         <v>1.5229999999999999</v>
       </c>
       <c r="AR21" s="3">
-        <v>0.039</v>
+        <v>3.9E-2</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>120</v>
       </c>
@@ -3546,10 +3522,10 @@
         <v>1.482</v>
       </c>
       <c r="AE22" s="4">
-        <v>7.7999999999999998</v>
+        <v>7.8</v>
       </c>
       <c r="AF22" s="4">
-        <v>5.2000000000000002</v>
+        <v>5.2</v>
       </c>
       <c r="AG22">
         <v>189</v>
@@ -3561,16 +3537,16 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="AJ22" s="4">
-        <v>9.9000000000000004</v>
+        <v>9.9</v>
       </c>
       <c r="AK22" s="3">
         <v>2.1429999999999998</v>
       </c>
       <c r="AL22" s="3">
-        <v>0.034000000000000002</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="AN22" s="4">
-        <v>23.600000000000001</v>
+        <v>23.6</v>
       </c>
       <c r="AO22" s="4">
         <v>19.399999999999999</v>
@@ -3582,995 +3558,12 @@
         <v>2.0430000000000001</v>
       </c>
       <c r="AR22" s="3">
-        <v>0.023</v>
+        <v>2.3E-2</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>122</v>
-      </c>
-      <c r="B23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" s="2">
-        <v>36.400660999999999</v>
-      </c>
-      <c r="F23" s="2">
-        <v>128.30723800000001</v>
-      </c>
-      <c r="G23" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" t="s">
-        <v>67</v>
-      </c>
-      <c r="L23" t="s">
-        <v>66</v>
-      </c>
-      <c r="M23" t="s">
-        <v>67</v>
-      </c>
-      <c r="N23" t="s">
-        <v>68</v>
-      </c>
-      <c r="O23" t="s">
-        <v>69</v>
-      </c>
-      <c r="P23" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>71</v>
-      </c>
-      <c r="R23" t="s">
-        <v>72</v>
-      </c>
-      <c r="S23" t="s">
-        <v>73</v>
-      </c>
-      <c r="T23" t="s">
-        <v>74</v>
-      </c>
-      <c r="U23" t="s">
-        <v>75</v>
-      </c>
-      <c r="V23" t="s">
-        <v>68</v>
-      </c>
-      <c r="W23" t="s">
-        <v>69</v>
-      </c>
-      <c r="X23" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>123</v>
-      </c>
-      <c r="AC23" s="3">
-        <v>0.062</v>
-      </c>
-      <c r="AD23" s="3">
-        <v>2.0449999999999999</v>
-      </c>
-      <c r="AE23" s="4">
-        <v>7.2999999999999998</v>
-      </c>
-      <c r="AF23" s="4">
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="AG23">
-        <v>127</v>
-      </c>
-      <c r="AH23" s="4">
-        <v>1.3999999999999999</v>
-      </c>
-      <c r="AI23" s="4">
-        <v>23.5</v>
-      </c>
-      <c r="AJ23" s="4">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="AK23" s="5">
-        <v>2.77</v>
-      </c>
-      <c r="AL23" s="3">
-        <v>0.086999999999999994</v>
-      </c>
-      <c r="AN23" s="4">
-        <v>20.300000000000001</v>
-      </c>
-      <c r="AO23" s="4">
-        <v>3.1000000000000001</v>
-      </c>
-      <c r="AP23" s="3">
-        <v>0.073999999999999996</v>
-      </c>
-      <c r="AQ23" s="3">
-        <v>2.7469999999999999</v>
-      </c>
-      <c r="AR23" s="3">
-        <v>0.079000000000000001</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="2">
-        <v>36.400660999999999</v>
-      </c>
-      <c r="F24" s="2">
-        <v>128.30723800000001</v>
-      </c>
-      <c r="G24" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24" t="s">
-        <v>67</v>
-      </c>
-      <c r="L24" t="s">
-        <v>66</v>
-      </c>
-      <c r="M24" t="s">
-        <v>67</v>
-      </c>
-      <c r="N24" t="s">
-        <v>68</v>
-      </c>
-      <c r="O24" t="s">
-        <v>69</v>
-      </c>
-      <c r="P24" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>71</v>
-      </c>
-      <c r="R24" t="s">
-        <v>72</v>
-      </c>
-      <c r="S24" t="s">
-        <v>73</v>
-      </c>
-      <c r="T24" t="s">
-        <v>74</v>
-      </c>
-      <c r="U24" t="s">
-        <v>75</v>
-      </c>
-      <c r="V24" t="s">
-        <v>68</v>
-      </c>
-      <c r="W24" t="s">
-        <v>69</v>
-      </c>
-      <c r="X24" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC24" s="3">
-        <v>0.056000000000000001</v>
-      </c>
-      <c r="AD24" s="3">
-        <v>2.4670000000000001</v>
-      </c>
-      <c r="AE24" s="4">
-        <v>7.2999999999999998</v>
-      </c>
-      <c r="AF24" s="4">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="AG24">
-        <v>183</v>
-      </c>
-      <c r="AH24" s="4">
-        <v>0.69999999999999996</v>
-      </c>
-      <c r="AI24">
-        <v>4</v>
-      </c>
-      <c r="AJ24" s="4">
-        <v>8.4000000000000004</v>
-      </c>
-      <c r="AK24" s="3">
-        <v>3.0409999999999999</v>
-      </c>
-      <c r="AL24" s="3">
-        <v>0.039</v>
-      </c>
-      <c r="AN24">
-        <v>24</v>
-      </c>
-      <c r="AO24" s="4">
-        <v>11.699999999999999</v>
-      </c>
-      <c r="AP24" s="3">
-        <v>0.027</v>
-      </c>
-      <c r="AQ24" s="3">
-        <v>3.012</v>
-      </c>
-      <c r="AR24" s="3">
-        <v>0.036999999999999998</v>
-      </c>
-      <c r="AS24" s="4">
-        <v>4.2000000000000002</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>126</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="2">
-        <v>36.400660999999999</v>
-      </c>
-      <c r="F25" s="2">
-        <v>128.30723800000001</v>
-      </c>
-      <c r="G25" t="s">
-        <v>66</v>
-      </c>
-      <c r="H25" t="s">
-        <v>67</v>
-      </c>
-      <c r="L25" t="s">
-        <v>66</v>
-      </c>
-      <c r="M25" t="s">
-        <v>67</v>
-      </c>
-      <c r="N25" t="s">
-        <v>68</v>
-      </c>
-      <c r="O25" t="s">
-        <v>69</v>
-      </c>
-      <c r="P25" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>71</v>
-      </c>
-      <c r="R25" t="s">
-        <v>72</v>
-      </c>
-      <c r="S25" t="s">
-        <v>73</v>
-      </c>
-      <c r="T25" t="s">
-        <v>74</v>
-      </c>
-      <c r="U25" t="s">
-        <v>75</v>
-      </c>
-      <c r="V25" t="s">
-        <v>68</v>
-      </c>
-      <c r="W25" t="s">
-        <v>69</v>
-      </c>
-      <c r="X25" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC25" s="3">
-        <v>0.062</v>
-      </c>
-      <c r="AD25" s="3">
-        <v>2.0339999999999998</v>
-      </c>
-      <c r="AE25" s="4">
-        <v>7.2999999999999998</v>
-      </c>
-      <c r="AF25" s="4">
-        <v>5.7000000000000002</v>
-      </c>
-      <c r="AG25">
-        <v>178</v>
-      </c>
-      <c r="AH25" s="4">
-        <v>1.7</v>
-      </c>
-      <c r="AI25" s="4">
-        <v>7.2000000000000002</v>
-      </c>
-      <c r="AJ25" s="4">
-        <v>8.4000000000000004</v>
-      </c>
-      <c r="AK25" s="3">
-        <v>2.7160000000000002</v>
-      </c>
-      <c r="AL25" s="3">
-        <v>0.065000000000000002</v>
-      </c>
-      <c r="AN25" s="4">
-        <v>26.100000000000001</v>
-      </c>
-      <c r="AO25" s="4">
-        <v>23.600000000000001</v>
-      </c>
-      <c r="AP25" s="5">
-        <v>0.050000000000000003</v>
-      </c>
-      <c r="AQ25" s="3">
-        <v>2.3639999999999999</v>
-      </c>
-      <c r="AR25" s="3">
-        <v>0.063</v>
-      </c>
-      <c r="AS25" s="4">
-        <v>4.2000000000000002</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>128</v>
-      </c>
-      <c r="B26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="2">
-        <v>36.400660999999999</v>
-      </c>
-      <c r="F26" s="2">
-        <v>128.30723800000001</v>
-      </c>
-      <c r="G26" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26" t="s">
-        <v>67</v>
-      </c>
-      <c r="L26" t="s">
-        <v>66</v>
-      </c>
-      <c r="M26" t="s">
-        <v>67</v>
-      </c>
-      <c r="N26" t="s">
-        <v>68</v>
-      </c>
-      <c r="O26" t="s">
-        <v>69</v>
-      </c>
-      <c r="P26" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>71</v>
-      </c>
-      <c r="R26" t="s">
-        <v>72</v>
-      </c>
-      <c r="S26" t="s">
-        <v>73</v>
-      </c>
-      <c r="T26" t="s">
-        <v>74</v>
-      </c>
-      <c r="U26" t="s">
-        <v>75</v>
-      </c>
-      <c r="V26" t="s">
-        <v>68</v>
-      </c>
-      <c r="W26" t="s">
-        <v>69</v>
-      </c>
-      <c r="X26" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>129</v>
-      </c>
-      <c r="AC26" s="5">
-        <v>0.050000000000000003</v>
-      </c>
-      <c r="AD26" s="3">
-        <v>1.637</v>
-      </c>
-      <c r="AE26" s="4">
-        <v>7.5999999999999996</v>
-      </c>
-      <c r="AF26" s="4">
-        <v>7.0999999999999996</v>
-      </c>
-      <c r="AG26">
-        <v>179</v>
-      </c>
-      <c r="AH26" s="4">
-        <v>2.7999999999999998</v>
-      </c>
-      <c r="AI26">
-        <v>14</v>
-      </c>
-      <c r="AJ26" s="4">
-        <v>8.9000000000000004</v>
-      </c>
-      <c r="AK26" s="3">
-        <v>2.089</v>
-      </c>
-      <c r="AL26" s="3">
-        <v>0.044999999999999998</v>
-      </c>
-      <c r="AN26" s="4">
-        <v>25.800000000000001</v>
-      </c>
-      <c r="AO26" s="4">
-        <v>38.100000000000001</v>
-      </c>
-      <c r="AP26" s="3">
-        <v>0.031</v>
-      </c>
-      <c r="AQ26" s="3">
-        <v>1.966</v>
-      </c>
-      <c r="AR26" s="3">
-        <v>0.043999999999999997</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>130</v>
-      </c>
-      <c r="B27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="2">
-        <v>36.400660999999999</v>
-      </c>
-      <c r="F27" s="2">
-        <v>128.30723800000001</v>
-      </c>
-      <c r="G27" t="s">
-        <v>66</v>
-      </c>
-      <c r="H27" t="s">
-        <v>67</v>
-      </c>
-      <c r="L27" t="s">
-        <v>66</v>
-      </c>
-      <c r="M27" t="s">
-        <v>67</v>
-      </c>
-      <c r="N27" t="s">
-        <v>68</v>
-      </c>
-      <c r="O27" t="s">
-        <v>69</v>
-      </c>
-      <c r="P27" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>71</v>
-      </c>
-      <c r="R27" t="s">
-        <v>72</v>
-      </c>
-      <c r="S27" t="s">
-        <v>73</v>
-      </c>
-      <c r="T27" t="s">
-        <v>74</v>
-      </c>
-      <c r="U27" t="s">
-        <v>75</v>
-      </c>
-      <c r="V27" t="s">
-        <v>68</v>
-      </c>
-      <c r="W27" t="s">
-        <v>69</v>
-      </c>
-      <c r="X27" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>131</v>
-      </c>
-      <c r="AC27" s="3">
-        <v>0.053999999999999999</v>
-      </c>
-      <c r="AD27" s="3">
-        <v>1.4890000000000001</v>
-      </c>
-      <c r="AE27" s="4">
-        <v>7.0999999999999996</v>
-      </c>
-      <c r="AF27" s="4">
-        <v>5.2000000000000002</v>
-      </c>
-      <c r="AG27">
-        <v>136</v>
-      </c>
-      <c r="AH27" s="4">
-        <v>0.90000000000000002</v>
-      </c>
-      <c r="AI27" s="4">
-        <v>18.800000000000001</v>
-      </c>
-      <c r="AJ27">
-        <v>8</v>
-      </c>
-      <c r="AK27" s="3">
-        <v>1.8660000000000001</v>
-      </c>
-      <c r="AL27" s="5">
-        <v>0.070000000000000007</v>
-      </c>
-      <c r="AN27" s="4">
-        <v>24.899999999999999</v>
-      </c>
-      <c r="AO27">
-        <v>7</v>
-      </c>
-      <c r="AP27" s="3">
-        <v>0.063</v>
-      </c>
-      <c r="AQ27" s="3">
-        <v>1.6859999999999999</v>
-      </c>
-      <c r="AR27" s="3">
-        <v>0.069000000000000006</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>132</v>
-      </c>
-      <c r="B28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="2">
-        <v>36.400660999999999</v>
-      </c>
-      <c r="F28" s="2">
-        <v>128.30723800000001</v>
-      </c>
-      <c r="G28" t="s">
-        <v>66</v>
-      </c>
-      <c r="H28" t="s">
-        <v>67</v>
-      </c>
-      <c r="L28" t="s">
-        <v>66</v>
-      </c>
-      <c r="M28" t="s">
-        <v>67</v>
-      </c>
-      <c r="N28" t="s">
-        <v>68</v>
-      </c>
-      <c r="O28" t="s">
-        <v>69</v>
-      </c>
-      <c r="P28" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>71</v>
-      </c>
-      <c r="R28" t="s">
-        <v>72</v>
-      </c>
-      <c r="S28" t="s">
-        <v>73</v>
-      </c>
-      <c r="T28" t="s">
-        <v>74</v>
-      </c>
-      <c r="U28" t="s">
-        <v>75</v>
-      </c>
-      <c r="V28" t="s">
-        <v>68</v>
-      </c>
-      <c r="W28" t="s">
-        <v>69</v>
-      </c>
-      <c r="X28" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>133</v>
-      </c>
-      <c r="AC28" s="3">
-        <v>0.042000000000000003</v>
-      </c>
-      <c r="AD28" s="3">
-        <v>1.385</v>
-      </c>
-      <c r="AE28" s="4">
-        <v>7.9000000000000004</v>
-      </c>
-      <c r="AF28">
-        <v>10</v>
-      </c>
-      <c r="AG28">
-        <v>110</v>
-      </c>
-      <c r="AH28" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="AI28" s="4">
-        <v>69.299999999999997</v>
-      </c>
-      <c r="AJ28" s="4">
-        <v>8.4000000000000004</v>
-      </c>
-      <c r="AK28" s="3">
-        <v>1.8819999999999999</v>
-      </c>
-      <c r="AL28" s="3">
-        <v>0.087999999999999995</v>
-      </c>
-      <c r="AN28" s="4">
-        <v>22.800000000000001</v>
-      </c>
-      <c r="AO28" s="4">
-        <v>3.6000000000000001</v>
-      </c>
-      <c r="AP28" s="3">
-        <v>0.070999999999999994</v>
-      </c>
-      <c r="AQ28" s="3">
-        <v>1.6879999999999999</v>
-      </c>
-      <c r="AR28" s="3">
-        <v>0.079000000000000001</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>134</v>
-      </c>
-      <c r="B29" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="2">
-        <v>36.400660999999999</v>
-      </c>
-      <c r="F29" s="2">
-        <v>128.30723800000001</v>
-      </c>
-      <c r="G29" t="s">
-        <v>66</v>
-      </c>
-      <c r="H29" t="s">
-        <v>67</v>
-      </c>
-      <c r="L29" t="s">
-        <v>66</v>
-      </c>
-      <c r="M29" t="s">
-        <v>67</v>
-      </c>
-      <c r="N29" t="s">
-        <v>68</v>
-      </c>
-      <c r="O29" t="s">
-        <v>69</v>
-      </c>
-      <c r="P29" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>71</v>
-      </c>
-      <c r="R29" t="s">
-        <v>72</v>
-      </c>
-      <c r="S29" t="s">
-        <v>73</v>
-      </c>
-      <c r="T29" t="s">
-        <v>74</v>
-      </c>
-      <c r="U29" t="s">
-        <v>75</v>
-      </c>
-      <c r="V29" t="s">
-        <v>68</v>
-      </c>
-      <c r="W29" t="s">
-        <v>69</v>
-      </c>
-      <c r="X29" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA29" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB29" t="s">
-        <v>135</v>
-      </c>
-      <c r="AC29" s="3">
-        <v>0.073999999999999996</v>
-      </c>
-      <c r="AD29" s="3">
-        <v>1.901</v>
-      </c>
-      <c r="AE29">
-        <v>8</v>
-      </c>
-      <c r="AF29" s="4">
-        <v>5.5</v>
-      </c>
-      <c r="AG29">
-        <v>165</v>
-      </c>
-      <c r="AH29" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="AI29" s="4">
-        <v>24.800000000000001</v>
-      </c>
-      <c r="AJ29" s="4">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="AK29" s="3">
-        <v>2.2839999999999998</v>
-      </c>
-      <c r="AL29" s="5">
-        <v>0.059999999999999998</v>
-      </c>
-      <c r="AN29" s="4">
-        <v>23.100000000000001</v>
-      </c>
-      <c r="AO29" s="4">
-        <v>3.6000000000000001</v>
-      </c>
-      <c r="AP29" s="3">
-        <v>0.033000000000000002</v>
-      </c>
-      <c r="AQ29" s="3">
-        <v>2.2679999999999998</v>
-      </c>
-      <c r="AR29" s="3">
-        <v>0.050999999999999997</v>
-      </c>
-      <c r="AS29" s="4">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>136</v>
-      </c>
-      <c r="B30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="2">
-        <v>36.400660999999999</v>
-      </c>
-      <c r="F30" s="2">
-        <v>128.30723800000001</v>
-      </c>
-      <c r="G30" t="s">
-        <v>66</v>
-      </c>
-      <c r="H30" t="s">
-        <v>67</v>
-      </c>
-      <c r="L30" t="s">
-        <v>66</v>
-      </c>
-      <c r="M30" t="s">
-        <v>67</v>
-      </c>
-      <c r="N30" t="s">
-        <v>68</v>
-      </c>
-      <c r="O30" t="s">
-        <v>69</v>
-      </c>
-      <c r="P30" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>71</v>
-      </c>
-      <c r="R30" t="s">
-        <v>72</v>
-      </c>
-      <c r="S30" t="s">
-        <v>73</v>
-      </c>
-      <c r="T30" t="s">
-        <v>74</v>
-      </c>
-      <c r="U30" t="s">
-        <v>75</v>
-      </c>
-      <c r="V30" t="s">
-        <v>68</v>
-      </c>
-      <c r="W30" t="s">
-        <v>69</v>
-      </c>
-      <c r="X30" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y30" t="s">
-        <v>76</v>
-      </c>
-      <c r="Z30" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA30" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>137</v>
-      </c>
-      <c r="AC30" s="3">
-        <v>0.106</v>
-      </c>
-      <c r="AD30" s="3">
-        <v>1.7410000000000001</v>
-      </c>
-      <c r="AE30" s="4">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="AF30" s="4">
-        <v>6.7999999999999998</v>
-      </c>
-      <c r="AG30">
-        <v>174</v>
-      </c>
-      <c r="AH30" s="4">
-        <v>1.2</v>
-      </c>
-      <c r="AI30" s="4">
-        <v>29.300000000000001</v>
-      </c>
-      <c r="AJ30" s="4">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="AK30" s="3">
-        <v>2.2549999999999999</v>
-      </c>
-      <c r="AL30" s="3">
-        <v>0.070999999999999994</v>
-      </c>
-      <c r="AN30" s="4">
-        <v>22.100000000000001</v>
-      </c>
-      <c r="AO30" s="4">
-        <v>9.0999999999999996</v>
-      </c>
-      <c r="AP30" s="3">
-        <v>0.042000000000000003</v>
-      </c>
-      <c r="AQ30" s="3">
-        <v>2.234</v>
-      </c>
-      <c r="AR30" s="3">
-        <v>0.050999999999999997</v>
-      </c>
-    </row>
-    <row r="31"/>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>